<commit_message>
Update: add direction of color of chart and map
</commit_message>
<xml_diff>
--- a/shared_data/social_codes.xlsx
+++ b/shared_data/social_codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>النشاط لدى الافراد البالغين 15 سنه فأكثر</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>Taux d’analphabétisme</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>down</t>
+  </si>
+  <si>
+    <t>direction</t>
   </si>
 </sst>
 </file>
@@ -551,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -564,7 +573,7 @@
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
@@ -574,8 +583,11 @@
       <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1">
+      <c r="D1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -585,8 +597,11 @@
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.2" thickBot="1">
+      <c r="D2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.2" thickBot="1">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
@@ -596,8 +611,11 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1">
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -607,8 +625,11 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1">
+      <c r="D4" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
@@ -618,8 +639,11 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1">
+      <c r="D5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
@@ -629,8 +653,11 @@
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.2" thickBot="1">
+      <c r="D6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.2" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -640,8 +667,11 @@
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.2" thickBot="1">
+      <c r="D7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.2" thickBot="1">
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
@@ -651,8 +681,11 @@
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.2" thickBot="1">
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.2" thickBot="1">
       <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
@@ -662,8 +695,11 @@
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1">
+      <c r="D9" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
@@ -673,8 +709,11 @@
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1">
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1">
       <c r="A11" s="4" t="s">
         <v>37</v>
       </c>
@@ -684,8 +723,11 @@
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1">
+      <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1">
       <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
@@ -695,8 +737,11 @@
       <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="28.2" thickBot="1">
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.2" thickBot="1">
       <c r="A13" s="4" t="s">
         <v>39</v>
       </c>
@@ -706,8 +751,11 @@
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1">
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
@@ -717,8 +765,11 @@
       <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1">
+      <c r="D14" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1">
       <c r="A15" s="4" t="s">
         <v>41</v>
       </c>
@@ -728,8 +779,11 @@
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1">
+      <c r="D15" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1">
       <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
@@ -738,6 +792,9 @@
       </c>
       <c r="C16" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: modifications of styles, adding groups of indices
</commit_message>
<xml_diff>
--- a/shared_data/social_codes.xlsx
+++ b/shared_data/social_codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
   <si>
     <t>النشاط لدى الافراد البالغين 15 سنه فأكثر</t>
   </si>
@@ -172,6 +172,105 @@
   </si>
   <si>
     <t>direction</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>alias_fr</t>
+  </si>
+  <si>
+    <t>alias_ar</t>
+  </si>
+  <si>
+    <t>Activité +15</t>
+  </si>
+  <si>
+    <t>النشاط +15</t>
+  </si>
+  <si>
+    <t>Chômage +15</t>
+  </si>
+  <si>
+    <t>البطالة +15</t>
+  </si>
+  <si>
+    <t>Handicap</t>
+  </si>
+  <si>
+    <t>الاعاقة</t>
+  </si>
+  <si>
+    <t>Pauvreté multidimensionnelle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> الفقر المتعدد الابعاد</t>
+  </si>
+  <si>
+    <t>Mortalité des enfants -5</t>
+  </si>
+  <si>
+    <t>وفيات الأطفال -5</t>
+  </si>
+  <si>
+    <t>Non-Scolarisation des enfants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عدم تمدرس الأطفال </t>
+  </si>
+  <si>
+    <t>Années de privation de scolarisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سنوات الحرمان التمدرس </t>
+  </si>
+  <si>
+    <t>Privation d'eau potable</t>
+  </si>
+  <si>
+    <t>Privation de l'électricité</t>
+  </si>
+  <si>
+    <t>Assainissement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Privation de logement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Privation en mode de cuisson </t>
+  </si>
+  <si>
+    <t xml:space="preserve">الحرمان من الكهرباء </t>
+  </si>
+  <si>
+    <t xml:space="preserve">الحرمان من الماء الصالح للشرب </t>
+  </si>
+  <si>
+    <t>الربط بشبكة التطهير</t>
+  </si>
+  <si>
+    <t>Réseau d’assainissement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الحرمان من السكن </t>
+  </si>
+  <si>
+    <t>الحرمان من نمط الطهي</t>
+  </si>
+  <si>
+    <t>Indices HCP</t>
+  </si>
+  <si>
+    <t>Indices Sectoriels</t>
+  </si>
+  <si>
+    <t>group_ar</t>
+  </si>
+  <si>
+    <t>المؤشرات المجالية</t>
+  </si>
+  <si>
+    <t>مؤشرات HCP</t>
   </si>
 </sst>
 </file>
@@ -201,7 +300,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -213,19 +312,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -267,19 +353,19 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,35 +646,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
     <col min="2" max="2" width="45.44140625" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="8" max="8" width="47.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1">
-      <c r="A2" s="4" t="s">
+      <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -600,9 +702,21 @@
       <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A3" s="4" t="s">
+      <c r="E2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -614,9 +728,21 @@
       <c r="D3" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1">
-      <c r="A4" s="4" t="s">
+      <c r="E3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -628,9 +754,21 @@
       <c r="D4" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1">
-      <c r="A5" s="4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -642,9 +780,21 @@
       <c r="D5" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1">
-      <c r="A6" s="4" t="s">
+      <c r="E5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -656,9 +806,21 @@
       <c r="D6" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A7" s="4" t="s">
+      <c r="E6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -670,9 +832,21 @@
       <c r="D7" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A8" s="4" t="s">
+      <c r="E7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -684,9 +858,21 @@
       <c r="D8" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A9" s="4" t="s">
+      <c r="E8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -698,9 +884,21 @@
       <c r="D9" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1">
-      <c r="A10" s="4" t="s">
+      <c r="E9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -712,9 +910,21 @@
       <c r="D10" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1">
-      <c r="A11" s="4" t="s">
+      <c r="E10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -726,9 +936,21 @@
       <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1">
-      <c r="A12" s="4" t="s">
+      <c r="E11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -740,9 +962,21 @@
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A13" s="4" t="s">
+      <c r="E12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -754,9 +988,21 @@
       <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1">
-      <c r="A14" s="4" t="s">
+      <c r="E13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -768,9 +1014,21 @@
       <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1">
-      <c r="A15" s="4" t="s">
+      <c r="E14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -782,20 +1040,50 @@
       <c r="D15" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1">
-      <c r="A16" s="4" t="s">
+      <c r="E15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.2" thickBot="1">
+      <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="D16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update: final hcp dashboard update 2025
</commit_message>
<xml_diff>
--- a/shared_data/social_codes.xlsx
+++ b/shared_data/social_codes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="7224" yWindow="684" windowWidth="22176" windowHeight="13176"/>
+    <workbookView xWindow="19092" yWindow="0" windowWidth="19416" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,17 +14,6 @@
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -65,24 +54,15 @@
     <t>HCP : pauvreté MD</t>
   </si>
   <si>
-    <t>populations légales</t>
-  </si>
-  <si>
     <t>Global</t>
   </si>
   <si>
     <t>Education</t>
   </si>
   <si>
-    <t>Sante</t>
-  </si>
-  <si>
     <t>Conditions de vie</t>
   </si>
   <si>
-    <t>dechets solide</t>
-  </si>
-  <si>
     <t>Scolarisation des enfants (privation)</t>
   </si>
   <si>
@@ -143,9 +123,6 @@
     <t>Lycée</t>
   </si>
   <si>
-    <t>education Supérieur</t>
-  </si>
-  <si>
     <t>تمدرس الأطفال (الحرمان)</t>
   </si>
   <si>
@@ -386,12 +363,6 @@
     <t>25</t>
   </si>
   <si>
-    <t>Pauvreté multidimensionnelle_2024</t>
-  </si>
-  <si>
-    <t>Pauvreté multidimensionnelle_2014</t>
-  </si>
-  <si>
     <t>الفقر متعدد الأبعاد(الحرمان)_2024</t>
   </si>
   <si>
@@ -419,18 +390,9 @@
     <t>Fos_Sept</t>
   </si>
   <si>
-    <t>Assain_liquide</t>
-  </si>
-  <si>
-    <t>Niveau_Scolaire</t>
-  </si>
-  <si>
     <t>HCP : Autres_Indicateurs</t>
   </si>
   <si>
-    <t>Education_Santé</t>
-  </si>
-  <si>
     <t>الشبكة العمومية للتطهير</t>
   </si>
   <si>
@@ -444,6 +406,33 @@
   </si>
   <si>
     <t>category</t>
+  </si>
+  <si>
+    <t>Pauvreté multidimensionnelle - 2024</t>
+  </si>
+  <si>
+    <t>Pauvreté multidimensionnelle -2014</t>
+  </si>
+  <si>
+    <t>Education Supérieur</t>
+  </si>
+  <si>
+    <t>Assainissement liquide</t>
+  </si>
+  <si>
+    <t>Education - Santé</t>
+  </si>
+  <si>
+    <t>Niveau scolaire</t>
+  </si>
+  <si>
+    <t>Santé</t>
+  </si>
+  <si>
+    <t>Dechets solide</t>
+  </si>
+  <si>
+    <t>Populations légales</t>
   </si>
 </sst>
 </file>
@@ -486,7 +475,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,6 +497,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -589,6 +584,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,7 +860,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -872,13 +870,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="45.44140625" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
@@ -902,7 +900,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
@@ -919,758 +917,758 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>136</v>
+        <v>115</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>136</v>
+        <v>34</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>136</v>
+        <v>35</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>136</v>
+        <v>36</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>14</v>
+        <v>135</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>136</v>
+        <v>37</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>14</v>
+        <v>135</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>135</v>
+        <v>38</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>135</v>
+        <v>39</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>135</v>
+        <v>40</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>135</v>
+        <v>41</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>135</v>
+        <v>42</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>135</v>
+        <v>43</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>135</v>
+        <v>44</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>135</v>
+        <v>45</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>135</v>
+        <v>46</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>135</v>
+      <c r="D17" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>135</v>
+      <c r="D18" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>135</v>
+        <v>46</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>135</v>
+        <v>47</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="5" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>135</v>
+        <v>48</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="5" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>135</v>
+        <v>49</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>135</v>
+        <v>50</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>135</v>
+        <v>51</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>135</v>
+        <v>52</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="8" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>135</v>
+        <v>53</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="8" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>135</v>
+        <v>54</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="8" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>135</v>
+        <v>55</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="8" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>135</v>
+        <v>56</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="8" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="3:3">

</xml_diff>